<commit_message>
Updated Planning and trello is updated
</commit_message>
<xml_diff>
--- a/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
+++ b/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2225" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2228" uniqueCount="660">
   <si>
     <t>Arne</t>
   </si>
@@ -4485,7 +4485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J371"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C335" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C320" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D355" sqref="D355"/>
     </sheetView>
   </sheetViews>
@@ -10410,8 +10410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y89"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="X28" sqref="X28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12166,12 +12166,12 @@
         <v>187</v>
       </c>
       <c r="J59" s="14"/>
+      <c r="L59" s="8" t="s">
+        <v>174</v>
+      </c>
       <c r="M59" s="23"/>
       <c r="N59" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="O59" s="8" t="s">
-        <v>174</v>
       </c>
       <c r="P59" s="14"/>
       <c r="Q59" s="8" t="s">
@@ -12204,12 +12204,12 @@
         <v>189</v>
       </c>
       <c r="J60" s="14"/>
+      <c r="L60" s="8" t="s">
+        <v>175</v>
+      </c>
       <c r="M60" s="23"/>
       <c r="N60" s="8" t="s">
         <v>121</v>
-      </c>
-      <c r="O60" s="8" t="s">
-        <v>175</v>
       </c>
       <c r="P60" s="14"/>
       <c r="Q60" s="8" t="s">
@@ -12236,12 +12236,12 @@
         <v>190</v>
       </c>
       <c r="J61" s="14"/>
+      <c r="L61" s="8" t="s">
+        <v>176</v>
+      </c>
       <c r="M61" s="23"/>
       <c r="N61" s="8" t="s">
         <v>122</v>
-      </c>
-      <c r="O61" s="8" t="s">
-        <v>176</v>
       </c>
       <c r="P61" s="14"/>
       <c r="Q61" s="8" t="s">
@@ -12266,6 +12266,9 @@
       <c r="G62" s="14"/>
       <c r="J62" s="14"/>
       <c r="M62" s="23"/>
+      <c r="N62" s="8" t="s">
+        <v>213</v>
+      </c>
       <c r="P62" s="14"/>
       <c r="Q62" s="8" t="s">
         <v>103</v>
@@ -12289,6 +12292,9 @@
       <c r="G63" s="14"/>
       <c r="J63" s="14"/>
       <c r="M63" s="23"/>
+      <c r="N63" s="8" t="s">
+        <v>214</v>
+      </c>
       <c r="P63" s="14"/>
       <c r="Q63" s="8" t="s">
         <v>305</v>
@@ -12312,6 +12318,9 @@
       <c r="G64" s="14"/>
       <c r="J64" s="14"/>
       <c r="M64" s="23"/>
+      <c r="N64" s="8" t="s">
+        <v>215</v>
+      </c>
       <c r="P64" s="14"/>
       <c r="R64" s="8" t="s">
         <v>293</v>

</xml_diff>

<commit_message>
Planning update and spirit particle
</commit_message>
<xml_diff>
--- a/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
+++ b/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2226" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2231" uniqueCount="664">
   <si>
     <t>Arne</t>
   </si>
@@ -2006,6 +2006,18 @@
   </si>
   <si>
     <t>SFX_GRAPPLINGHOOK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirit </t>
+  </si>
+  <si>
+    <t>9_ENEMY_SPIRIT</t>
+  </si>
+  <si>
+    <t>Alieke &amp; Marc</t>
+  </si>
+  <si>
+    <t>9P_ENEMY_SPIRIT</t>
   </si>
 </sst>
 </file>
@@ -4517,10 +4529,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J371"/>
+  <dimension ref="A1:J372"/>
   <sheetViews>
-    <sheetView topLeftCell="C320" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D355" sqref="D355"/>
+    <sheetView tabSelected="1" topLeftCell="A340" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H370" sqref="H370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10238,7 +10250,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="353" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A353" s="14"/>
       <c r="B353" s="14"/>
       <c r="C353" t="s">
@@ -10248,11 +10260,11 @@
         <v>655</v>
       </c>
     </row>
-    <row r="354" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A354" s="14"/>
       <c r="B354" s="14"/>
     </row>
-    <row r="355" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A355" s="14"/>
       <c r="B355" s="7" t="s">
         <v>397</v>
@@ -10261,7 +10273,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="356" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A356" s="14"/>
       <c r="B356" s="14"/>
       <c r="C356" t="s">
@@ -10274,7 +10286,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="357" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A357" s="14"/>
       <c r="B357" s="14"/>
       <c r="C357" t="s">
@@ -10287,7 +10299,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="358" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A358" s="14"/>
       <c r="B358" s="14"/>
       <c r="C358" t="s">
@@ -10300,7 +10312,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="359" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A359" s="14"/>
       <c r="B359" s="14"/>
       <c r="C359" t="s">
@@ -10313,7 +10325,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="360" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A360" s="14"/>
       <c r="B360" s="14"/>
       <c r="C360" t="s">
@@ -10326,7 +10338,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="361" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A361" s="14"/>
       <c r="B361" s="14"/>
       <c r="C361" t="s">
@@ -10336,11 +10348,11 @@
         <v>653</v>
       </c>
     </row>
-    <row r="362" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A362" s="14"/>
       <c r="B362" s="14"/>
     </row>
-    <row r="363" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A363" s="14"/>
       <c r="B363" t="s">
         <v>573</v>
@@ -10349,7 +10361,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="364" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A364" s="14"/>
       <c r="B364" s="14"/>
       <c r="C364" t="s">
@@ -10362,7 +10374,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="365" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A365" s="14"/>
       <c r="B365" s="14"/>
       <c r="C365" t="s">
@@ -10375,7 +10387,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="366" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A366" s="14"/>
       <c r="B366" s="14"/>
       <c r="C366" t="s">
@@ -10391,48 +10403,64 @@
         <v>468</v>
       </c>
     </row>
-    <row r="367" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A367" s="14"/>
       <c r="B367" s="14"/>
-    </row>
-    <row r="368" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C367" t="s">
+        <v>660</v>
+      </c>
+      <c r="D367" t="s">
+        <v>661</v>
+      </c>
+      <c r="H367" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="368" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A368" s="14"/>
-      <c r="B368" t="s">
+      <c r="B368" s="14"/>
+    </row>
+    <row r="369" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A369" s="14"/>
+      <c r="B369" t="s">
         <v>42</v>
       </c>
-      <c r="C368" t="s">
+      <c r="C369" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="369" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A369" s="14"/>
-      <c r="B369" s="14"/>
-      <c r="C369" t="s">
-        <v>310</v>
-      </c>
-      <c r="D369" t="s">
-        <v>311</v>
-      </c>
-      <c r="G369" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="370" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A370" s="14"/>
       <c r="B370" s="14"/>
       <c r="C370" t="s">
-        <v>650</v>
+        <v>310</v>
       </c>
       <c r="D370" t="s">
-        <v>651</v>
+        <v>311</v>
       </c>
       <c r="G370" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="371" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H370" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A371" s="14"/>
       <c r="B371" s="14"/>
+      <c r="C371" t="s">
+        <v>650</v>
+      </c>
+      <c r="D371" t="s">
+        <v>651</v>
+      </c>
+      <c r="G371" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A372" s="14"/>
+      <c r="B372" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10444,8 +10472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="N63" sqref="N63"/>
+    <sheetView topLeftCell="F1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10618,6 +10646,9 @@
         <v>641</v>
       </c>
       <c r="M3" s="23"/>
+      <c r="N3" s="20" t="s">
+        <v>663</v>
+      </c>
       <c r="P3" s="14"/>
       <c r="S3" s="14"/>
       <c r="V3" s="14"/>

</xml_diff>

<commit_message>
Planning update and particles
</commit_message>
<xml_diff>
--- a/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
+++ b/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2231" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2232" uniqueCount="664">
   <si>
     <t>Arne</t>
   </si>
@@ -4532,7 +4532,7 @@
   <dimension ref="A1:J372"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A340" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H370" sqref="H370"/>
+      <selection activeCell="H364" sqref="H364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10197,6 +10197,9 @@
       <c r="G348" t="s">
         <v>468</v>
       </c>
+      <c r="H348" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="349" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A349" s="14"/>
@@ -10311,6 +10314,9 @@
       <c r="G358" t="s">
         <v>468</v>
       </c>
+      <c r="H358" t="s">
+        <v>662</v>
+      </c>
     </row>
     <row r="359" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A359" s="14"/>
@@ -10420,7 +10426,7 @@
       <c r="A368" s="14"/>
       <c r="B368" s="14"/>
     </row>
-    <row r="369" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A369" s="14"/>
       <c r="B369" t="s">
         <v>42</v>
@@ -10429,7 +10435,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="370" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A370" s="14"/>
       <c r="B370" s="14"/>
       <c r="C370" t="s">
@@ -10441,11 +10447,8 @@
       <c r="G370" t="s">
         <v>468</v>
       </c>
-      <c r="H370" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="371" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A371" s="14"/>
       <c r="B371" s="14"/>
       <c r="C371" t="s">
@@ -10458,7 +10461,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A372" s="14"/>
       <c r="B372" s="14"/>
     </row>

</xml_diff>

<commit_message>
Planning, Particles and metadata
</commit_message>
<xml_diff>
--- a/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
+++ b/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2248" uniqueCount="668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2249" uniqueCount="668">
   <si>
     <t>Arne</t>
   </si>
@@ -10514,8 +10514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L2" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10857,6 +10857,9 @@
         <v>379</v>
       </c>
       <c r="M11" s="23"/>
+      <c r="N11" s="20" t="s">
+        <v>651</v>
+      </c>
       <c r="P11" s="14"/>
       <c r="S11" s="14"/>
       <c r="V11" s="14"/>

</xml_diff>

<commit_message>
Planning update and personal scene
</commit_message>
<xml_diff>
--- a/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
+++ b/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2153" uniqueCount="711">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2156" uniqueCount="712">
   <si>
     <t>Arne</t>
   </si>
@@ -2159,6 +2159,9 @@
   </si>
   <si>
     <t>3D_KAPPAK_TERRAIN</t>
+  </si>
+  <si>
+    <t>Arne &amp; Janneke</t>
   </si>
 </sst>
 </file>
@@ -4726,8 +4729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G410"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A376" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D383" sqref="D383"/>
+    <sheetView topLeftCell="A341" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D374" sqref="D374"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9803,7 +9806,7 @@
         <v>466</v>
       </c>
       <c r="G354" t="s">
-        <v>0</v>
+        <v>711</v>
       </c>
     </row>
     <row r="355" spans="1:7" x14ac:dyDescent="0.25">
@@ -9864,7 +9867,7 @@
         <v>466</v>
       </c>
       <c r="G359" t="s">
-        <v>1</v>
+        <v>661</v>
       </c>
     </row>
     <row r="360" spans="1:7" x14ac:dyDescent="0.25">
@@ -9880,7 +9883,7 @@
         <v>466</v>
       </c>
       <c r="G360" t="s">
-        <v>1</v>
+        <v>661</v>
       </c>
     </row>
     <row r="361" spans="1:7" x14ac:dyDescent="0.25">
@@ -9912,7 +9915,7 @@
         <v>466</v>
       </c>
       <c r="G362" t="s">
-        <v>1</v>
+        <v>661</v>
       </c>
     </row>
     <row r="363" spans="1:7" x14ac:dyDescent="0.25">
@@ -9944,7 +9947,7 @@
         <v>466</v>
       </c>
       <c r="G364" t="s">
-        <v>0</v>
+        <v>711</v>
       </c>
     </row>
     <row r="365" spans="1:7" x14ac:dyDescent="0.25">
@@ -10002,7 +10005,7 @@
         <v>466</v>
       </c>
       <c r="G369" t="s">
-        <v>1</v>
+        <v>661</v>
       </c>
     </row>
     <row r="370" spans="1:7" x14ac:dyDescent="0.25">
@@ -10063,7 +10066,7 @@
         <v>466</v>
       </c>
       <c r="G374" t="s">
-        <v>0</v>
+        <v>711</v>
       </c>
     </row>
     <row r="375" spans="1:7" x14ac:dyDescent="0.25">
@@ -10404,8 +10407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y89"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" topLeftCell="D26" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="M63" sqref="M63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12610,7 +12613,9 @@
       <c r="N70" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="O70" s="8"/>
+      <c r="O70" s="8" t="s">
+        <v>582</v>
+      </c>
       <c r="Q70" s="8" t="s">
         <v>101</v>
       </c>
@@ -12637,7 +12642,9 @@
       <c r="K71" s="8"/>
       <c r="L71" s="8"/>
       <c r="N71" s="8"/>
-      <c r="O71" s="8"/>
+      <c r="O71" s="8" t="s">
+        <v>589</v>
+      </c>
       <c r="Q71" s="8" t="s">
         <v>303</v>
       </c>
@@ -12664,7 +12671,9 @@
       <c r="K72" s="8"/>
       <c r="L72" s="8"/>
       <c r="N72" s="8"/>
-      <c r="O72" s="8"/>
+      <c r="O72" s="8" t="s">
+        <v>648</v>
+      </c>
       <c r="Q72" s="8"/>
       <c r="R72" s="8" t="s">
         <v>291</v>

</xml_diff>

<commit_message>
Kart Added to Excel
</commit_message>
<xml_diff>
--- a/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
+++ b/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2183" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2186" uniqueCount="724">
   <si>
     <t>Arne</t>
   </si>
@@ -2158,12 +2158,6 @@
     <t>Arne &amp; Janneke</t>
   </si>
   <si>
-    <t>KartItemBox.cs</t>
-  </si>
-  <si>
-    <t>8S_KAPPAK_ITEMBOX</t>
-  </si>
-  <si>
     <t>2D_CHAR_MCMODEL</t>
   </si>
   <si>
@@ -2192,6 +2186,18 @@
   </si>
   <si>
     <t>4U_ENV_STEPPINGSTONE</t>
+  </si>
+  <si>
+    <t>Kart</t>
+  </si>
+  <si>
+    <t>3D_KAPPAK_KART</t>
+  </si>
+  <si>
+    <t>2D_KAPPAK_KART</t>
+  </si>
+  <si>
+    <t>4U_KAPPAK_KART</t>
   </si>
 </sst>
 </file>
@@ -4724,10 +4730,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G415"/>
+  <dimension ref="A1:G416"/>
   <sheetViews>
-    <sheetView topLeftCell="A168" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G192" sqref="G192"/>
+    <sheetView tabSelected="1" topLeftCell="A375" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D394" sqref="D394"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5419,10 +5425,10 @@
       <c r="A44" s="14"/>
       <c r="B44" s="14"/>
       <c r="C44" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="D44" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="F44" t="s">
         <v>465</v>
@@ -5435,10 +5441,10 @@
       <c r="A45" s="14"/>
       <c r="B45" s="14"/>
       <c r="C45" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="D45" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="F45" t="s">
         <v>458</v>
@@ -6633,20 +6639,20 @@
       <c r="A123" s="14"/>
       <c r="B123" s="14"/>
       <c r="C123" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="D123" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="14"/>
       <c r="B124" s="14"/>
       <c r="C124" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="D124" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -7615,10 +7621,10 @@
       <c r="A190" s="14"/>
       <c r="B190" s="14"/>
       <c r="C190" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="D190" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="F190" t="s">
         <v>465</v>
@@ -7631,10 +7637,10 @@
       <c r="A191" s="14"/>
       <c r="B191" s="14"/>
       <c r="C191" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="D191" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="F191" t="s">
         <v>464</v>
@@ -10175,208 +10181,202 @@
         <v>707</v>
       </c>
     </row>
-    <row r="385" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A385" s="14"/>
       <c r="B385" s="14"/>
-    </row>
-    <row r="386" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C385" t="s">
+        <v>720</v>
+      </c>
+      <c r="D385" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="386" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A386" s="14"/>
-      <c r="B386" t="s">
+      <c r="B386" s="14"/>
+    </row>
+    <row r="387" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A387" s="14"/>
+      <c r="B387" t="s">
         <v>26</v>
       </c>
-      <c r="C386" t="s">
+      <c r="C387" t="s">
         <v>672</v>
       </c>
     </row>
-    <row r="387" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A387" s="14"/>
-      <c r="B387" s="14"/>
-      <c r="C387" t="s">
-        <v>702</v>
-      </c>
-      <c r="D387" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="388" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A388" s="14"/>
       <c r="B388" s="14"/>
       <c r="C388" t="s">
-        <v>205</v>
+        <v>702</v>
       </c>
       <c r="D388" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="389" spans="1:7" x14ac:dyDescent="0.25">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="389" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A389" s="14"/>
       <c r="B389" s="14"/>
-    </row>
-    <row r="390" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C389" t="s">
+        <v>205</v>
+      </c>
+      <c r="D389" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="390" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A390" s="14"/>
       <c r="B390" s="14"/>
-    </row>
-    <row r="391" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C390" t="s">
+        <v>720</v>
+      </c>
+      <c r="D390" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="391" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A391" s="14"/>
-      <c r="B391" t="s">
+      <c r="B391" s="14"/>
+    </row>
+    <row r="392" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A392" s="14"/>
+      <c r="B392" t="s">
         <v>27</v>
       </c>
-      <c r="C391" t="s">
+      <c r="C392" t="s">
         <v>673</v>
       </c>
-      <c r="D391" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="392" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A392" s="14"/>
-      <c r="B392" s="14"/>
-      <c r="C392" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="393" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="393" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A393" s="14"/>
       <c r="B393" s="14"/>
-    </row>
-    <row r="394" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C393" t="s">
+        <v>702</v>
+      </c>
+      <c r="D393" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="394" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A394" s="14"/>
-      <c r="B394" t="s">
-        <v>670</v>
-      </c>
+      <c r="B394" s="14"/>
       <c r="C394" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="395" spans="1:7" x14ac:dyDescent="0.25">
+        <v>720</v>
+      </c>
+      <c r="D394" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="395" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A395" s="14"/>
       <c r="B395" s="14"/>
     </row>
-    <row r="396" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A396" s="14"/>
-      <c r="B396" s="14"/>
-    </row>
-    <row r="397" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B396" t="s">
+        <v>670</v>
+      </c>
+      <c r="C396" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="397" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A397" s="14"/>
       <c r="B397" s="14"/>
     </row>
-    <row r="398" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A398" s="14"/>
       <c r="B398" s="14"/>
     </row>
-    <row r="399" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A399" s="14"/>
-      <c r="B399" t="s">
-        <v>669</v>
-      </c>
-      <c r="C399" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="400" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B399" s="14"/>
+    </row>
+    <row r="400" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A400" s="14"/>
       <c r="B400" s="14"/>
-      <c r="C400" t="s">
-        <v>682</v>
-      </c>
-      <c r="D400" t="s">
-        <v>700</v>
-      </c>
-      <c r="F400" t="s">
-        <v>465</v>
-      </c>
-      <c r="G400" t="s">
-        <v>664</v>
-      </c>
     </row>
     <row r="401" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A401" s="14"/>
-      <c r="B401" s="14"/>
+      <c r="B401" t="s">
+        <v>669</v>
+      </c>
       <c r="C401" t="s">
-        <v>683</v>
-      </c>
-      <c r="D401" t="s">
-        <v>699</v>
-      </c>
-      <c r="F401" t="s">
-        <v>465</v>
-      </c>
-      <c r="G401" t="s">
-        <v>1</v>
+        <v>675</v>
       </c>
     </row>
     <row r="402" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A402" s="14"/>
       <c r="B402" s="14"/>
       <c r="C402" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="D402" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="F402" t="s">
         <v>465</v>
       </c>
       <c r="G402" t="s">
-        <v>1</v>
+        <v>664</v>
       </c>
     </row>
     <row r="403" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A403" s="14"/>
       <c r="B403" s="14"/>
       <c r="C403" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="D403" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="F403" t="s">
         <v>465</v>
       </c>
       <c r="G403" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="404" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A404" s="14"/>
       <c r="B404" s="14"/>
       <c r="C404" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="D404" t="s">
-        <v>692</v>
+        <v>698</v>
       </c>
       <c r="F404" t="s">
         <v>465</v>
       </c>
       <c r="G404" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="405" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A405" s="14"/>
       <c r="B405" s="14"/>
       <c r="C405" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D405" t="s">
-        <v>693</v>
+        <v>697</v>
       </c>
       <c r="F405" t="s">
         <v>465</v>
       </c>
       <c r="G405" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="406" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A406" s="14"/>
       <c r="B406" s="14"/>
       <c r="C406" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="D406" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="F406" t="s">
         <v>465</v>
@@ -10389,58 +10389,58 @@
       <c r="A407" s="14"/>
       <c r="B407" s="14"/>
       <c r="C407" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="D407" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="F407" t="s">
         <v>465</v>
       </c>
       <c r="G407" t="s">
-        <v>664</v>
+        <v>1</v>
       </c>
     </row>
     <row r="408" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A408" s="14"/>
       <c r="B408" s="14"/>
       <c r="C408" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="D408" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="F408" t="s">
         <v>465</v>
       </c>
       <c r="G408" t="s">
-        <v>664</v>
+        <v>0</v>
       </c>
     </row>
     <row r="409" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A409" s="14"/>
       <c r="B409" s="14"/>
       <c r="C409" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="D409" t="s">
-        <v>701</v>
+        <v>695</v>
       </c>
       <c r="F409" t="s">
         <v>465</v>
       </c>
       <c r="G409" t="s">
-        <v>1</v>
+        <v>664</v>
       </c>
     </row>
     <row r="410" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A410" s="14"/>
       <c r="B410" s="14"/>
       <c r="C410" t="s">
-        <v>710</v>
+        <v>690</v>
       </c>
       <c r="D410" t="s">
-        <v>711</v>
+        <v>696</v>
       </c>
       <c r="F410" t="s">
         <v>465</v>
@@ -10451,16 +10451,28 @@
     </row>
     <row r="411" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A411" s="14"/>
-      <c r="B411" t="s">
-        <v>31</v>
-      </c>
+      <c r="B411" s="14"/>
       <c r="C411" t="s">
-        <v>676</v>
+        <v>691</v>
+      </c>
+      <c r="D411" t="s">
+        <v>701</v>
+      </c>
+      <c r="F411" t="s">
+        <v>465</v>
+      </c>
+      <c r="G411" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="412" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A412" s="14"/>
-      <c r="B412" s="14"/>
+      <c r="B412" t="s">
+        <v>31</v>
+      </c>
+      <c r="C412" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="413" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A413" s="14"/>
@@ -10473,6 +10485,10 @@
     <row r="415" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A415" s="14"/>
       <c r="B415" s="14"/>
+    </row>
+    <row r="416" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A416" s="14"/>
+      <c r="B416" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10484,8 +10500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G25" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="Q56" sqref="Q56"/>
+    <sheetView topLeftCell="P1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10737,6 +10753,9 @@
         <v>701</v>
       </c>
       <c r="S4" s="14"/>
+      <c r="T4" s="20" t="s">
+        <v>693</v>
+      </c>
       <c r="V4" s="14"/>
       <c r="Y4" s="14"/>
       <c r="Z4" s="27"/>
@@ -12325,7 +12344,7 @@
         <v>200</v>
       </c>
       <c r="R46" s="8" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="S46" s="14"/>
       <c r="T46" s="8" t="s">
@@ -12380,7 +12399,7 @@
         <v>224</v>
       </c>
       <c r="R47" s="8" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="S47" s="14"/>
       <c r="T47" s="8" t="s">
@@ -12432,7 +12451,7 @@
         <v>318</v>
       </c>
       <c r="R48" s="8" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="S48" s="14"/>
       <c r="T48" s="8" t="s">
@@ -12528,7 +12547,7 @@
       </c>
       <c r="S50" s="14"/>
       <c r="T50" s="8" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="U50" s="8" t="s">
         <v>344</v>
@@ -12574,7 +12593,7 @@
       </c>
       <c r="S51" s="14"/>
       <c r="T51" s="8" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="U51" s="8" t="s">
         <v>343</v>
@@ -12612,7 +12631,7 @@
       <c r="P52" s="14"/>
       <c r="S52" s="14"/>
       <c r="T52" s="8" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="V52" s="14"/>
       <c r="Y52" s="14"/>
@@ -13284,7 +13303,7 @@
         <v>217</v>
       </c>
       <c r="Q66" s="8" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="R66" s="8" t="s">
         <v>291</v>

</xml_diff>

<commit_message>
KART Has really been added now
</commit_message>
<xml_diff>
--- a/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
+++ b/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2186" uniqueCount="724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2189" uniqueCount="724">
   <si>
     <t>Arne</t>
   </si>
@@ -4732,7 +4732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G416"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A375" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A375" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D394" sqref="D394"/>
     </sheetView>
   </sheetViews>
@@ -10500,8 +10500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ89"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView tabSelected="1" topLeftCell="Q31" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="T46" sqref="T46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12228,7 +12228,7 @@
       </c>
       <c r="S44" s="14"/>
       <c r="T44" s="8" t="s">
-        <v>252</v>
+        <v>722</v>
       </c>
       <c r="U44" s="8" t="s">
         <v>325</v>
@@ -12287,7 +12287,7 @@
         <v>287</v>
       </c>
       <c r="T45" s="8" t="s">
-        <v>253</v>
+        <v>721</v>
       </c>
       <c r="U45" s="8" t="s">
         <v>327</v>
@@ -12348,7 +12348,7 @@
       </c>
       <c r="S46" s="14"/>
       <c r="T46" s="8" t="s">
-        <v>254</v>
+        <v>723</v>
       </c>
       <c r="U46" s="8" t="s">
         <v>332</v>
@@ -12499,6 +12499,9 @@
       <c r="Q49" s="8" t="s">
         <v>635</v>
       </c>
+      <c r="R49" s="8" t="s">
+        <v>252</v>
+      </c>
       <c r="S49" s="14"/>
       <c r="T49" s="8" t="s">
         <v>78</v>
@@ -12545,6 +12548,9 @@
       <c r="Q50" s="8" t="s">
         <v>317</v>
       </c>
+      <c r="R50" s="8" t="s">
+        <v>253</v>
+      </c>
       <c r="S50" s="14"/>
       <c r="T50" s="8" t="s">
         <v>712</v>
@@ -12590,6 +12596,9 @@
       <c r="P51" s="14"/>
       <c r="Q51" s="8" t="s">
         <v>319</v>
+      </c>
+      <c r="R51" s="8" t="s">
+        <v>254</v>
       </c>
       <c r="S51" s="14"/>
       <c r="T51" s="8" t="s">

</xml_diff>

<commit_message>
Planning updated and scripting
</commit_message>
<xml_diff>
--- a/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
+++ b/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2189" uniqueCount="724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2189" uniqueCount="723">
   <si>
     <t>Arne</t>
   </si>
@@ -1559,9 +1559,6 @@
   </si>
   <si>
     <t>WEEK 49</t>
-  </si>
-  <si>
-    <t>WEEK 52</t>
   </si>
   <si>
     <t>WEEK 50</t>
@@ -3152,10 +3149,10 @@
         <v>477</v>
       </c>
       <c r="CJ2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="EU2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="3" spans="1:151" x14ac:dyDescent="0.25">
@@ -3181,10 +3178,10 @@
         <v>477</v>
       </c>
       <c r="CJ3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="EU3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="4" spans="1:151" x14ac:dyDescent="0.25">
@@ -3210,10 +3207,10 @@
         <v>477</v>
       </c>
       <c r="CJ4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="EU4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="5" spans="1:151" x14ac:dyDescent="0.25">
@@ -3239,15 +3236,15 @@
         <v>477</v>
       </c>
       <c r="CJ5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="EU5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="6" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B6" s="2">
         <v>0.61458333333333337</v>
@@ -3256,7 +3253,7 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E6">
         <v>13</v>
@@ -3271,10 +3268,10 @@
     <row r="7" spans="1:151" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="CJ7" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="EU7" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="8" spans="1:151" x14ac:dyDescent="0.25">
@@ -3282,10 +3279,10 @@
         <v>4</v>
       </c>
       <c r="CJ8" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="EU8" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="9" spans="1:151" x14ac:dyDescent="0.25">
@@ -3311,10 +3308,10 @@
         <v>477</v>
       </c>
       <c r="CJ9" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="EU9" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="10" spans="1:151" x14ac:dyDescent="0.25">
@@ -3340,10 +3337,10 @@
         <v>477</v>
       </c>
       <c r="CJ10" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="EU10" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="11" spans="1:151" x14ac:dyDescent="0.25">
@@ -3369,10 +3366,10 @@
         <v>477</v>
       </c>
       <c r="CJ11" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="EU11" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="12" spans="1:151" x14ac:dyDescent="0.25">
@@ -3947,7 +3944,7 @@
         <v>11</v>
       </c>
       <c r="CJ13" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="CN13" s="1" t="s">
         <v>11</v>
@@ -4034,7 +4031,7 @@
         <v>11</v>
       </c>
       <c r="EU13" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="14" spans="1:151" x14ac:dyDescent="0.25">
@@ -4066,13 +4063,13 @@
         <v>13</v>
       </c>
       <c r="CJ14" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="ES14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="EU14" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="15" spans="1:151" x14ac:dyDescent="0.25">
@@ -4125,7 +4122,7 @@
         <v>451</v>
       </c>
       <c r="CJ15" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="CP15" t="s">
         <v>452</v>
@@ -4146,7 +4143,7 @@
         <v>457</v>
       </c>
       <c r="EU15" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="16" spans="1:151" x14ac:dyDescent="0.25">
@@ -4172,435 +4169,435 @@
         <v>477</v>
       </c>
       <c r="J16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="M16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="N16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="O16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="P16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="Q16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="R16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="S16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="T16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="U16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="V16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="W16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="X16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="Y16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="Z16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AA16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AB16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AC16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AD16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AE16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AF16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AG16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AH16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AI16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AJ16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AK16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AL16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AM16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AN16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AO16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AP16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AQ16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AR16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AS16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AT16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AU16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AV16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AW16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AX16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AY16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AZ16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BA16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BB16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BC16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BD16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BE16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BF16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BG16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BH16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BI16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BJ16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BK16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BL16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BM16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BN16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BO16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BP16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BQ16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BR16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BS16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BT16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BU16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BV16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BW16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BX16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BY16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="BZ16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CA16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CB16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CC16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CD16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CE16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CF16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CG16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CH16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CI16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CJ16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CK16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CL16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CM16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CN16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CO16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CP16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CQ16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CR16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CS16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CT16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CU16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CV16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CW16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CX16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CY16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="CZ16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DA16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DB16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DC16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DD16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DE16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DF16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DG16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DH16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DI16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DJ16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DK16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DL16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DM16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DN16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DO16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DP16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DQ16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DR16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DS16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DT16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DU16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DV16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DW16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DX16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DY16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="DZ16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="EA16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="EB16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="EC16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="ED16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="EE16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="EF16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="EG16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="EH16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="EI16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="EJ16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="EK16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="EL16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="EM16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="EN16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="EO16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="EP16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="EQ16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="ER16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="ES16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="ET16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="EU16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B17" s="2">
         <v>0.61458333333333337</v>
@@ -4609,7 +4606,7 @@
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E17">
         <v>13</v>
@@ -5121,7 +5118,7 @@
         <v>139</v>
       </c>
       <c r="D25" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F25" t="s">
         <v>464</v>
@@ -5425,10 +5422,10 @@
       <c r="A44" s="14"/>
       <c r="B44" s="14"/>
       <c r="C44" t="s">
+        <v>710</v>
+      </c>
+      <c r="D44" t="s">
         <v>711</v>
-      </c>
-      <c r="D44" t="s">
-        <v>712</v>
       </c>
       <c r="F44" t="s">
         <v>465</v>
@@ -5441,10 +5438,10 @@
       <c r="A45" s="14"/>
       <c r="B45" s="14"/>
       <c r="C45" t="s">
+        <v>712</v>
+      </c>
+      <c r="D45" t="s">
         <v>713</v>
-      </c>
-      <c r="D45" t="s">
-        <v>714</v>
       </c>
       <c r="F45" t="s">
         <v>458</v>
@@ -5460,7 +5457,7 @@
         <v>207</v>
       </c>
       <c r="D46" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F46" t="s">
         <v>458</v>
@@ -5476,7 +5473,7 @@
         <v>208</v>
       </c>
       <c r="D47" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F47" t="s">
         <v>458</v>
@@ -5492,7 +5489,7 @@
         <v>209</v>
       </c>
       <c r="D48" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F48" t="s">
         <v>458</v>
@@ -6054,20 +6051,20 @@
       <c r="A83" s="14"/>
       <c r="B83" s="14"/>
       <c r="C83" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D83" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="14"/>
       <c r="B84" s="14"/>
       <c r="C84" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="D84" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -6332,10 +6329,10 @@
       <c r="A103" s="14"/>
       <c r="B103" s="14"/>
       <c r="C103" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D103" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F103" t="s">
         <v>464</v>
@@ -6639,20 +6636,20 @@
       <c r="A123" s="14"/>
       <c r="B123" s="14"/>
       <c r="C123" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D123" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="14"/>
       <c r="B124" s="14"/>
       <c r="C124" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D124" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -6870,10 +6867,10 @@
       <c r="A138" s="14"/>
       <c r="B138" s="14"/>
       <c r="C138" t="s">
+        <v>677</v>
+      </c>
+      <c r="D138" t="s">
         <v>678</v>
-      </c>
-      <c r="D138" t="s">
-        <v>679</v>
       </c>
       <c r="F138" t="s">
         <v>458</v>
@@ -7368,10 +7365,10 @@
       <c r="A173" s="14"/>
       <c r="B173" s="14"/>
       <c r="C173" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D173" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F173" t="s">
         <v>464</v>
@@ -7621,10 +7618,10 @@
       <c r="A190" s="14"/>
       <c r="B190" s="14"/>
       <c r="C190" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D190" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="F190" t="s">
         <v>465</v>
@@ -7637,10 +7634,10 @@
       <c r="A191" s="14"/>
       <c r="B191" s="14"/>
       <c r="C191" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D191" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="F191" t="s">
         <v>464</v>
@@ -7800,10 +7797,10 @@
       <c r="A201" s="14"/>
       <c r="B201" s="14"/>
       <c r="C201" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="D201" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="202" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8242,10 +8239,10 @@
       <c r="A234" s="14"/>
       <c r="B234" s="14"/>
       <c r="C234" t="s">
+        <v>631</v>
+      </c>
+      <c r="D234" t="s">
         <v>632</v>
-      </c>
-      <c r="D234" t="s">
-        <v>633</v>
       </c>
       <c r="F234" t="s">
         <v>458</v>
@@ -8258,10 +8255,10 @@
       <c r="A235" s="14"/>
       <c r="B235" s="14"/>
       <c r="C235" t="s">
+        <v>633</v>
+      </c>
+      <c r="D235" t="s">
         <v>634</v>
-      </c>
-      <c r="D235" t="s">
-        <v>635</v>
       </c>
       <c r="F235" t="s">
         <v>458</v>
@@ -8521,10 +8518,10 @@
       <c r="A249" s="14"/>
       <c r="B249" s="14"/>
       <c r="C249" t="s">
+        <v>650</v>
+      </c>
+      <c r="D249" t="s">
         <v>651</v>
-      </c>
-      <c r="D249" t="s">
-        <v>652</v>
       </c>
       <c r="F249" t="s">
         <v>458</v>
@@ -8684,7 +8681,7 @@
         <v>406</v>
       </c>
       <c r="C263" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="E263" t="s">
         <v>437</v>
@@ -8700,7 +8697,7 @@
       <c r="A264" s="14"/>
       <c r="B264" s="14"/>
       <c r="C264" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="F264" t="s">
         <v>458</v>
@@ -8710,7 +8707,7 @@
       <c r="A265" s="14"/>
       <c r="B265" s="14"/>
       <c r="C265" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="F265" t="s">
         <v>464</v>
@@ -8720,7 +8717,7 @@
       <c r="A266" s="14"/>
       <c r="B266" s="14"/>
       <c r="C266" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="F266" t="s">
         <v>464</v>
@@ -8938,10 +8935,10 @@
       <c r="A283" s="14"/>
       <c r="B283" s="14"/>
       <c r="C283" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="F283" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G283" t="s">
         <v>2</v>
@@ -9158,7 +9155,7 @@
         <v>464</v>
       </c>
       <c r="G301" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="302" spans="1:7" x14ac:dyDescent="0.25">
@@ -9178,7 +9175,7 @@
       <c r="A303" s="14"/>
       <c r="B303" s="14"/>
       <c r="C303" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="F303" t="s">
         <v>464</v>
@@ -9188,7 +9185,7 @@
       <c r="A304" s="14"/>
       <c r="B304" s="14"/>
       <c r="C304" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F304" t="s">
         <v>464</v>
@@ -9198,7 +9195,7 @@
       <c r="A305" s="14"/>
       <c r="B305" s="14"/>
       <c r="C305" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="F305" t="s">
         <v>464</v>
@@ -9391,7 +9388,7 @@
       <c r="A321" s="14"/>
       <c r="B321" s="14"/>
       <c r="C321" s="4" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F321" t="s">
         <v>458</v>
@@ -9404,7 +9401,7 @@
       <c r="A322" s="14"/>
       <c r="B322" s="14"/>
       <c r="C322" s="4" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F322" t="s">
         <v>458</v>
@@ -9417,7 +9414,7 @@
       <c r="A323" s="14"/>
       <c r="B323" s="14"/>
       <c r="C323" s="4" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F323" t="s">
         <v>458</v>
@@ -9430,7 +9427,7 @@
       <c r="A324" s="14"/>
       <c r="B324" s="14"/>
       <c r="C324" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F324" t="s">
         <v>458</v>
@@ -9702,7 +9699,7 @@
       <c r="A346" s="14"/>
       <c r="B346" s="14"/>
       <c r="C346" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F346" t="s">
         <v>458</v>
@@ -9787,7 +9784,7 @@
       <c r="A353" s="14"/>
       <c r="B353" s="15"/>
       <c r="C353" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F353" t="s">
         <v>458</v>
@@ -9823,13 +9820,13 @@
         <v>303</v>
       </c>
       <c r="E356" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F356" t="s">
         <v>464</v>
       </c>
       <c r="G356" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="357" spans="1:7" x14ac:dyDescent="0.25">
@@ -9845,71 +9842,71 @@
         <v>464</v>
       </c>
       <c r="G357" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="358" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A358" s="14"/>
       <c r="B358" s="14"/>
       <c r="C358" t="s">
+        <v>576</v>
+      </c>
+      <c r="D358" t="s">
         <v>577</v>
-      </c>
-      <c r="D358" t="s">
-        <v>578</v>
       </c>
       <c r="F358" t="s">
         <v>464</v>
       </c>
       <c r="G358" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="359" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A359" s="14"/>
       <c r="B359" s="14"/>
       <c r="C359" t="s">
+        <v>578</v>
+      </c>
+      <c r="D359" t="s">
         <v>579</v>
-      </c>
-      <c r="D359" t="s">
-        <v>580</v>
       </c>
       <c r="F359" t="s">
         <v>464</v>
       </c>
       <c r="G359" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="360" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A360" s="14"/>
       <c r="B360" s="14"/>
       <c r="C360" t="s">
+        <v>580</v>
+      </c>
+      <c r="D360" t="s">
         <v>581</v>
-      </c>
-      <c r="D360" t="s">
-        <v>582</v>
       </c>
       <c r="F360" t="s">
         <v>464</v>
       </c>
       <c r="G360" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="361" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A361" s="14"/>
       <c r="B361" s="14"/>
       <c r="C361" t="s">
+        <v>648</v>
+      </c>
+      <c r="D361" t="s">
         <v>649</v>
-      </c>
-      <c r="D361" t="s">
-        <v>650</v>
       </c>
       <c r="F361" t="s">
         <v>464</v>
       </c>
       <c r="G361" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="362" spans="1:7" x14ac:dyDescent="0.25">
@@ -9922,39 +9919,39 @@
         <v>393</v>
       </c>
       <c r="C363" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="364" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A364" s="14"/>
       <c r="B364" s="14"/>
       <c r="C364" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D364" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F364" t="s">
         <v>464</v>
       </c>
       <c r="G364" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="365" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A365" s="14"/>
       <c r="B365" s="14"/>
       <c r="C365" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D365" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F365" t="s">
         <v>464</v>
       </c>
       <c r="G365" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="366" spans="1:7" x14ac:dyDescent="0.25">
@@ -9964,39 +9961,39 @@
         <v>273</v>
       </c>
       <c r="D366" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F366" t="s">
         <v>464</v>
       </c>
       <c r="G366" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="367" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A367" s="14"/>
       <c r="B367" s="14"/>
       <c r="C367" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D367" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F367" t="s">
         <v>464</v>
       </c>
       <c r="G367" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="368" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A368" s="14"/>
       <c r="B368" s="14"/>
       <c r="C368" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D368" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F368" t="s">
         <v>464</v>
@@ -10006,19 +10003,19 @@
       <c r="A369" s="14"/>
       <c r="B369" s="14"/>
       <c r="C369" t="s">
+        <v>646</v>
+      </c>
+      <c r="D369" t="s">
         <v>647</v>
       </c>
-      <c r="D369" t="s">
-        <v>648</v>
-      </c>
       <c r="E369" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="F369" t="s">
         <v>464</v>
       </c>
       <c r="G369" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="370" spans="1:7" x14ac:dyDescent="0.25">
@@ -10028,20 +10025,20 @@
     <row r="371" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A371" s="14"/>
       <c r="B371" t="s">
+        <v>567</v>
+      </c>
+      <c r="C371" t="s">
         <v>568</v>
-      </c>
-      <c r="C371" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="372" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A372" s="14"/>
       <c r="B372" s="14"/>
       <c r="C372" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D372" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F372" t="s">
         <v>464</v>
@@ -10051,10 +10048,10 @@
       <c r="A373" s="14"/>
       <c r="B373" s="14"/>
       <c r="C373" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D373" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F373" t="s">
         <v>464</v>
@@ -10064,35 +10061,35 @@
       <c r="A374" s="14"/>
       <c r="B374" s="14"/>
       <c r="C374" t="s">
+        <v>574</v>
+      </c>
+      <c r="D374" t="s">
         <v>575</v>
       </c>
-      <c r="D374" t="s">
-        <v>576</v>
-      </c>
       <c r="E374" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F374" t="s">
         <v>464</v>
       </c>
       <c r="G374" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="375" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A375" s="14"/>
       <c r="B375" s="14"/>
       <c r="C375" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D375" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F375" t="s">
         <v>464</v>
       </c>
       <c r="G375" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="376" spans="1:7" x14ac:dyDescent="0.25">
@@ -10121,23 +10118,23 @@
         <v>464</v>
       </c>
       <c r="G378" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="379" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A379" s="14"/>
       <c r="B379" s="14"/>
       <c r="C379" t="s">
+        <v>644</v>
+      </c>
+      <c r="D379" t="s">
         <v>645</v>
-      </c>
-      <c r="D379" t="s">
-        <v>646</v>
       </c>
       <c r="F379" t="s">
         <v>464</v>
       </c>
       <c r="G379" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="380" spans="1:7" x14ac:dyDescent="0.25">
@@ -10146,10 +10143,10 @@
     </row>
     <row r="381" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A381" s="26" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C381" s="26" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="382" spans="1:7" x14ac:dyDescent="0.25">
@@ -10158,37 +10155,37 @@
         <v>25</v>
       </c>
       <c r="C382" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="383" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A383" s="14"/>
       <c r="B383" s="14"/>
       <c r="C383" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D383" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="384" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A384" s="14"/>
       <c r="B384" s="14"/>
       <c r="C384" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D384" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A385" s="14"/>
       <c r="B385" s="14"/>
       <c r="C385" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D385" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.25">
@@ -10201,17 +10198,17 @@
         <v>26</v>
       </c>
       <c r="C387" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A388" s="14"/>
       <c r="B388" s="14"/>
       <c r="C388" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D388" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.25">
@@ -10221,17 +10218,17 @@
         <v>205</v>
       </c>
       <c r="D389" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A390" s="14"/>
       <c r="B390" s="14"/>
       <c r="C390" t="s">
+        <v>719</v>
+      </c>
+      <c r="D390" t="s">
         <v>720</v>
-      </c>
-      <c r="D390" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.25">
@@ -10244,27 +10241,27 @@
         <v>27</v>
       </c>
       <c r="C392" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A393" s="14"/>
       <c r="B393" s="14"/>
       <c r="C393" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D393" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A394" s="14"/>
       <c r="B394" s="14"/>
       <c r="C394" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D394" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.25">
@@ -10274,10 +10271,10 @@
     <row r="396" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A396" s="14"/>
       <c r="B396" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C396" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.25">
@@ -10299,36 +10296,36 @@
     <row r="401" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A401" s="14"/>
       <c r="B401" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C401" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="402" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A402" s="14"/>
       <c r="B402" s="14"/>
       <c r="C402" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D402" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="F402" t="s">
         <v>465</v>
       </c>
       <c r="G402" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="403" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A403" s="14"/>
       <c r="B403" s="14"/>
       <c r="C403" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D403" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="F403" t="s">
         <v>465</v>
@@ -10341,10 +10338,10 @@
       <c r="A404" s="14"/>
       <c r="B404" s="14"/>
       <c r="C404" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D404" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="F404" t="s">
         <v>465</v>
@@ -10357,10 +10354,10 @@
       <c r="A405" s="14"/>
       <c r="B405" s="14"/>
       <c r="C405" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D405" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="F405" t="s">
         <v>465</v>
@@ -10373,10 +10370,10 @@
       <c r="A406" s="14"/>
       <c r="B406" s="14"/>
       <c r="C406" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="D406" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="F406" t="s">
         <v>465</v>
@@ -10389,10 +10386,10 @@
       <c r="A407" s="14"/>
       <c r="B407" s="14"/>
       <c r="C407" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D407" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="F407" t="s">
         <v>465</v>
@@ -10405,10 +10402,10 @@
       <c r="A408" s="14"/>
       <c r="B408" s="14"/>
       <c r="C408" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D408" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="F408" t="s">
         <v>465</v>
@@ -10421,42 +10418,42 @@
       <c r="A409" s="14"/>
       <c r="B409" s="14"/>
       <c r="C409" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D409" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="F409" t="s">
         <v>465</v>
       </c>
       <c r="G409" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="410" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A410" s="14"/>
       <c r="B410" s="14"/>
       <c r="C410" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D410" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="F410" t="s">
         <v>465</v>
       </c>
       <c r="G410" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="411" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A411" s="14"/>
       <c r="B411" s="14"/>
       <c r="C411" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D411" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="F411" t="s">
         <v>465</v>
@@ -10471,7 +10468,7 @@
         <v>31</v>
       </c>
       <c r="C412" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="413" spans="1:7" x14ac:dyDescent="0.25">
@@ -10500,8 +10497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q31" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="T46" sqref="T46"/>
+    <sheetView tabSelected="1" topLeftCell="Q37" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="R65" sqref="R65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10560,7 +10557,7 @@
         <v>450</v>
       </c>
       <c r="M1" s="23" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="N1" t="s">
         <v>451</v>
@@ -10584,7 +10581,7 @@
         <v>457</v>
       </c>
       <c r="X1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="2" spans="1:36" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10603,7 +10600,7 @@
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="19" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I2" s="19" t="s">
         <v>505</v>
@@ -10627,21 +10624,21 @@
         <v>510</v>
       </c>
       <c r="R2" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="S2" s="19"/>
       <c r="T2" s="19" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="U2" s="19" t="s">
-        <v>511</v>
+        <v>500</v>
       </c>
       <c r="V2" s="19"/>
       <c r="W2" s="19" t="s">
-        <v>500</v>
+        <v>445</v>
       </c>
       <c r="X2" s="19" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="Z2" s="27"/>
       <c r="AA2" s="16"/>
@@ -10667,45 +10664,45 @@
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="25" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" s="20" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="J3" s="14"/>
       <c r="K3" s="20" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="L3" s="20" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="M3" s="23"/>
       <c r="N3" s="20" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="O3" s="20" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="20" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="S3" s="14"/>
       <c r="T3" s="20" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="U3" s="20" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="V3" s="14"/>
       <c r="Y3" s="14"/>
@@ -10731,30 +10728,30 @@
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="25" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="20" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="J4" s="14"/>
       <c r="M4" s="23"/>
       <c r="N4" s="20" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="O4" s="20" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="P4" s="14"/>
       <c r="R4" s="20" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="S4" s="14"/>
       <c r="T4" s="20" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="V4" s="14"/>
       <c r="Y4" s="14"/>
@@ -10780,19 +10777,19 @@
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="25" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="G5" s="14"/>
       <c r="J5" s="14"/>
       <c r="M5" s="23"/>
       <c r="N5" s="20" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="O5" s="20" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="P5" s="14"/>
       <c r="S5" s="14"/>
@@ -10820,10 +10817,10 @@
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="25" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G6" s="14"/>
       <c r="J6" s="14"/>
@@ -10832,7 +10829,7 @@
         <v>303</v>
       </c>
       <c r="O6" s="20" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="P6" s="14"/>
       <c r="S6" s="14"/>
@@ -10857,7 +10854,7 @@
       <c r="J7" s="14"/>
       <c r="M7" s="23"/>
       <c r="N7" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="P7" s="14"/>
       <c r="S7" s="14"/>
@@ -10955,35 +10952,35 @@
         <v>382</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="J11" s="14"/>
       <c r="K11" s="20" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="L11" s="20" t="s">
         <v>375</v>
       </c>
       <c r="M11" s="23"/>
       <c r="N11" s="20" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="O11" s="20" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="P11" s="14"/>
       <c r="Q11" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="R11" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="S11" s="14"/>
       <c r="T11" s="20" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="U11" s="20" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="V11" s="14"/>
       <c r="Y11" s="14"/>
@@ -11012,15 +11009,15 @@
       <c r="J12" s="14"/>
       <c r="M12" s="23"/>
       <c r="O12" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="P12" s="14"/>
       <c r="S12" s="14"/>
       <c r="T12" s="20" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="U12" s="20" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="V12" s="14"/>
       <c r="Y12" s="14"/>
@@ -11168,52 +11165,52 @@
         <v>2</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D19" s="14"/>
       <c r="E19" s="20" t="s">
         <v>359</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="20" t="s">
         <v>368</v>
       </c>
       <c r="I19" s="20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="J19" s="14"/>
       <c r="K19" s="20" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="L19" s="20" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="M19" s="23"/>
       <c r="N19" s="20" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="O19" s="20" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="P19" s="14"/>
       <c r="Q19" s="20" t="s">
+        <v>610</v>
+      </c>
+      <c r="R19" s="20" t="s">
         <v>611</v>
-      </c>
-      <c r="R19" s="20" t="s">
-        <v>612</v>
       </c>
       <c r="S19" s="14"/>
       <c r="T19" s="20" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="U19" s="20" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="V19" s="14"/>
       <c r="Y19" s="14"/>
@@ -11232,52 +11229,52 @@
     <row r="20" spans="1:36" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="20" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="20" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F20" s="20" t="s">
         <v>369</v>
       </c>
       <c r="G20" s="14"/>
       <c r="H20" s="20" t="s">
+        <v>621</v>
+      </c>
+      <c r="I20" s="20" t="s">
         <v>622</v>
-      </c>
-      <c r="I20" s="20" t="s">
-        <v>623</v>
       </c>
       <c r="J20" s="14"/>
       <c r="K20" s="20" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="L20" s="20" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="M20" s="23"/>
       <c r="N20" s="20" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="O20" s="20" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="P20" s="14"/>
       <c r="Q20" s="20" t="s">
+        <v>612</v>
+      </c>
+      <c r="R20" s="20" t="s">
         <v>613</v>
-      </c>
-      <c r="R20" s="20" t="s">
-        <v>614</v>
       </c>
       <c r="S20" s="14"/>
       <c r="T20" s="20" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="U20" s="20" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="V20" s="14"/>
       <c r="Y20" s="14"/>
@@ -11296,14 +11293,14 @@
     <row r="21" spans="1:36" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="20" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D21" s="14"/>
       <c r="F21" s="20" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="G21" s="14"/>
       <c r="J21" s="14"/>
@@ -11339,14 +11336,14 @@
     <row r="22" spans="1:36" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="20" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D22" s="14"/>
       <c r="G22" s="14"/>
       <c r="J22" s="14"/>
       <c r="M22" s="23"/>
       <c r="N22" s="20" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="P22" s="14"/>
       <c r="S22" s="14"/>
@@ -11367,14 +11364,14 @@
     <row r="23" spans="1:36" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="20" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D23" s="14"/>
       <c r="G23" s="14"/>
       <c r="J23" s="14"/>
       <c r="M23" s="23"/>
       <c r="N23" s="20" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="P23" s="14"/>
       <c r="S23" s="14"/>
@@ -11395,7 +11392,7 @@
     <row r="24" spans="1:36" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="20" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D24" s="14"/>
       <c r="G24" s="14"/>
@@ -11420,7 +11417,7 @@
     <row r="25" spans="1:36" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="20" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>359</v>
@@ -11461,31 +11458,31 @@
     </row>
     <row r="27" spans="1:36" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D27" s="14"/>
       <c r="G27" s="14"/>
       <c r="J27" s="14"/>
       <c r="M27" s="23"/>
       <c r="N27" s="20" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="O27" s="20" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="P27" s="14"/>
       <c r="Q27" s="20" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="R27" s="20" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="S27" s="14"/>
       <c r="T27" s="20" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="U27" s="20" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="V27" s="14"/>
       <c r="Y27" s="14"/>
@@ -11508,18 +11505,18 @@
       <c r="J28" s="14"/>
       <c r="M28" s="23"/>
       <c r="N28" s="20" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="O28" s="20" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="P28" s="14"/>
       <c r="S28" s="14"/>
       <c r="T28" s="20" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="U28" s="20" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="V28" s="14"/>
       <c r="Y28" s="14"/>
@@ -11542,7 +11539,7 @@
       <c r="J29" s="14"/>
       <c r="M29" s="23"/>
       <c r="N29" s="20" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="P29" s="14"/>
       <c r="S29" s="14"/>
@@ -11567,7 +11564,7 @@
       <c r="J30" s="14"/>
       <c r="M30" s="23"/>
       <c r="N30" s="20" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="P30" s="14"/>
       <c r="S30" s="14"/>
@@ -11592,7 +11589,7 @@
       <c r="J31" s="14"/>
       <c r="M31" s="23"/>
       <c r="N31" s="20" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="P31" s="14"/>
       <c r="S31" s="14"/>
@@ -11617,7 +11614,7 @@
       <c r="J32" s="14"/>
       <c r="M32" s="23"/>
       <c r="N32" s="20" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="P32" s="14"/>
       <c r="S32" s="14"/>
@@ -11650,7 +11647,7 @@
       <c r="L33" s="20"/>
       <c r="M33" s="23"/>
       <c r="N33" s="20" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="O33" s="20"/>
       <c r="P33" s="14"/>
@@ -11694,24 +11691,24 @@
         <v>398</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D35" s="14"/>
       <c r="E35" s="20" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G35" s="14"/>
       <c r="H35" s="20" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="I35" s="20" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="J35" s="14"/>
       <c r="K35" s="20" t="s">
@@ -11743,10 +11740,10 @@
       </c>
       <c r="V35" s="14"/>
       <c r="W35" s="20" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X35" s="20" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="Y35" s="14"/>
       <c r="Z35" s="27"/>
@@ -11764,34 +11761,34 @@
     <row r="36" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="20" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D36" s="14"/>
       <c r="E36" s="20"/>
       <c r="F36" s="20"/>
       <c r="G36" s="14"/>
       <c r="H36" s="20" t="s">
+        <v>618</v>
+      </c>
+      <c r="I36" s="20" t="s">
         <v>619</v>
-      </c>
-      <c r="I36" s="20" t="s">
-        <v>620</v>
       </c>
       <c r="J36" s="14"/>
       <c r="K36" s="20" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="L36" s="20" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="M36" s="23"/>
       <c r="N36" s="20" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="O36" s="20" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="P36" s="14"/>
       <c r="Q36" s="20" t="s">
@@ -11802,14 +11799,14 @@
       </c>
       <c r="S36" s="14"/>
       <c r="T36" s="20" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="U36" s="20" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="V36" s="14"/>
       <c r="W36" s="20" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="X36" s="20"/>
       <c r="Y36" s="14"/>
@@ -11838,7 +11835,7 @@
       <c r="F37" s="20"/>
       <c r="G37" s="14"/>
       <c r="H37" s="20" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I37" s="20"/>
       <c r="J37" s="14"/>
@@ -11850,10 +11847,10 @@
       </c>
       <c r="M37" s="23"/>
       <c r="N37" s="20" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="O37" s="20" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="P37" s="14"/>
       <c r="Q37" s="20"/>
@@ -11865,7 +11862,7 @@
       <c r="U37" s="20"/>
       <c r="V37" s="14"/>
       <c r="W37" s="20" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="X37" s="20"/>
       <c r="Y37" s="14"/>
@@ -11903,7 +11900,7 @@
       <c r="M38" s="23"/>
       <c r="N38" s="20"/>
       <c r="O38" s="20" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="P38" s="14"/>
       <c r="Q38" s="20"/>
@@ -11945,7 +11942,7 @@
       <c r="M39" s="23"/>
       <c r="N39" s="20"/>
       <c r="O39" s="20" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="P39" s="14"/>
       <c r="Q39" s="20"/>
@@ -12122,7 +12119,7 @@
         <v>7</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>219</v>
@@ -12150,24 +12147,24 @@
       </c>
       <c r="M43" s="23"/>
       <c r="N43" s="8" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="O43" s="8" t="s">
         <v>179</v>
       </c>
       <c r="P43" s="14"/>
       <c r="Q43" s="8" t="s">
-        <v>180</v>
+        <v>204</v>
       </c>
       <c r="R43" s="8" t="s">
-        <v>283</v>
+        <v>713</v>
       </c>
       <c r="S43" s="14"/>
       <c r="T43" s="8" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="U43" s="8" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="V43" s="14"/>
       <c r="Y43" s="14"/>
@@ -12186,7 +12183,7 @@
     <row r="44" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="8" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>221</v>
@@ -12214,21 +12211,21 @@
       </c>
       <c r="M44" s="23"/>
       <c r="N44" s="8" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="O44" s="8" t="s">
         <v>318</v>
       </c>
       <c r="P44" s="14"/>
       <c r="Q44" s="8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="R44" s="8" t="s">
-        <v>285</v>
+        <v>715</v>
       </c>
       <c r="S44" s="14"/>
       <c r="T44" s="8" t="s">
-        <v>722</v>
+        <v>79</v>
       </c>
       <c r="U44" s="8" t="s">
         <v>325</v>
@@ -12250,16 +12247,16 @@
     <row r="45" spans="1:36" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="8" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>229</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H45" s="8" t="s">
         <v>337</v>
@@ -12268,26 +12265,26 @@
         <v>337</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="L45" s="8" t="s">
         <v>69</v>
       </c>
       <c r="M45" s="23"/>
       <c r="N45" s="8" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="O45" s="8" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="Q45" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="R45" s="8" t="s">
-        <v>287</v>
+        <v>718</v>
       </c>
       <c r="T45" s="8" t="s">
-        <v>721</v>
+        <v>77</v>
       </c>
       <c r="U45" s="8" t="s">
         <v>327</v>
@@ -12341,17 +12338,17 @@
       </c>
       <c r="P46" s="14"/>
       <c r="Q46" s="8" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
       <c r="R46" s="8" t="s">
-        <v>714</v>
+        <v>252</v>
       </c>
       <c r="S46" s="14"/>
       <c r="T46" s="8" t="s">
-        <v>723</v>
+        <v>78</v>
       </c>
       <c r="U46" s="8" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="V46" s="14"/>
       <c r="Y46" s="14"/>
@@ -12370,7 +12367,7 @@
     <row r="47" spans="1:36" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="8" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>228</v>
@@ -12396,17 +12393,17 @@
       </c>
       <c r="P47" s="14"/>
       <c r="Q47" s="8" t="s">
-        <v>224</v>
+        <v>318</v>
       </c>
       <c r="R47" s="8" t="s">
-        <v>716</v>
+        <v>253</v>
       </c>
       <c r="S47" s="14"/>
       <c r="T47" s="8" t="s">
-        <v>79</v>
+        <v>711</v>
       </c>
       <c r="U47" s="8" t="s">
-        <v>333</v>
+        <v>344</v>
       </c>
       <c r="V47" s="14"/>
       <c r="Y47" s="14"/>
@@ -12425,7 +12422,7 @@
     <row r="48" spans="1:36" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="8" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>438</v>
@@ -12436,29 +12433,32 @@
         <v>157</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="J48" s="14"/>
       <c r="L48" s="8" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="M48" s="23"/>
       <c r="N48" s="8" t="s">
         <v>162</v>
       </c>
+      <c r="O48" s="8" t="s">
+        <v>283</v>
+      </c>
       <c r="P48" s="14"/>
       <c r="Q48" s="8" t="s">
-        <v>318</v>
+        <v>634</v>
       </c>
       <c r="R48" s="8" t="s">
-        <v>719</v>
+        <v>254</v>
       </c>
       <c r="S48" s="14"/>
       <c r="T48" s="8" t="s">
-        <v>77</v>
+        <v>714</v>
       </c>
       <c r="U48" s="8" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="V48" s="14"/>
       <c r="Y48" s="14"/>
@@ -12485,7 +12485,7 @@
       <c r="D49" s="14"/>
       <c r="G49" s="14"/>
       <c r="H49" s="8" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I49" s="8" t="s">
         <v>493</v>
@@ -12495,19 +12495,22 @@
       <c r="N49" s="8" t="s">
         <v>316</v>
       </c>
+      <c r="O49" s="8" t="s">
+        <v>285</v>
+      </c>
       <c r="P49" s="14"/>
       <c r="Q49" s="8" t="s">
-        <v>635</v>
+        <v>317</v>
       </c>
       <c r="R49" s="8" t="s">
-        <v>252</v>
+        <v>721</v>
       </c>
       <c r="S49" s="14"/>
       <c r="T49" s="8" t="s">
-        <v>78</v>
+        <v>716</v>
       </c>
       <c r="U49" s="8" t="s">
-        <v>339</v>
+        <v>98</v>
       </c>
       <c r="V49" s="14"/>
       <c r="Y49" s="14"/>
@@ -12526,7 +12529,7 @@
     <row r="50" spans="1:36" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="8" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>440</v>
@@ -12544,19 +12547,22 @@
       <c r="N50" s="8" t="s">
         <v>314</v>
       </c>
+      <c r="O50" s="8" t="s">
+        <v>287</v>
+      </c>
       <c r="P50" s="14"/>
       <c r="Q50" s="8" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="R50" s="8" t="s">
-        <v>253</v>
+        <v>720</v>
       </c>
       <c r="S50" s="14"/>
       <c r="T50" s="8" t="s">
-        <v>712</v>
+        <v>324</v>
       </c>
       <c r="U50" s="8" t="s">
-        <v>344</v>
+        <v>97</v>
       </c>
       <c r="V50" s="14"/>
       <c r="Y50" s="14"/>
@@ -12575,10 +12581,10 @@
     <row r="51" spans="1:36" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="8" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D51" s="22"/>
       <c r="G51" s="14"/>
@@ -12593,19 +12599,19 @@
       <c r="N51" s="8" t="s">
         <v>315</v>
       </c>
+      <c r="O51" s="8" t="s">
+        <v>180</v>
+      </c>
       <c r="P51" s="14"/>
-      <c r="Q51" s="8" t="s">
-        <v>319</v>
-      </c>
       <c r="R51" s="8" t="s">
-        <v>254</v>
+        <v>722</v>
       </c>
       <c r="S51" s="14"/>
       <c r="T51" s="8" t="s">
-        <v>715</v>
+        <v>332</v>
       </c>
       <c r="U51" s="8" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="V51" s="14"/>
       <c r="Y51" s="14"/>
@@ -12624,7 +12630,7 @@
     <row r="52" spans="1:36" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="8" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C52" s="21"/>
       <c r="D52" s="22"/>
@@ -12635,12 +12641,12 @@
       <c r="J52" s="14"/>
       <c r="M52" s="23"/>
       <c r="N52" s="8" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="P52" s="14"/>
       <c r="S52" s="14"/>
       <c r="T52" s="8" t="s">
-        <v>717</v>
+        <v>721</v>
       </c>
       <c r="V52" s="14"/>
       <c r="Y52" s="14"/>
@@ -12720,7 +12726,7 @@
       </c>
       <c r="J54" s="14"/>
       <c r="K54" s="8" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="L54" s="8" t="s">
         <v>347</v>
@@ -12737,7 +12743,7 @@
         <v>72</v>
       </c>
       <c r="R54" s="8" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="S54" s="14"/>
       <c r="T54" s="8" t="s">
@@ -12763,7 +12769,7 @@
     <row r="55" spans="1:36" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="8" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>354</v>
@@ -12781,7 +12787,7 @@
         <v>243</v>
       </c>
       <c r="K55" s="8" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="L55" s="8"/>
       <c r="M55" s="23"/>
@@ -12795,7 +12801,7 @@
         <v>75</v>
       </c>
       <c r="R55" s="8" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="T55" s="8" t="s">
         <v>300</v>
@@ -12838,7 +12844,7 @@
       </c>
       <c r="J56" s="14"/>
       <c r="K56" s="8" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="M56" s="23"/>
       <c r="N56" s="8" t="s">
@@ -12852,11 +12858,11 @@
         <v>74</v>
       </c>
       <c r="R56" s="8" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="S56" s="14"/>
       <c r="T56" s="8" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="V56" s="14"/>
       <c r="Y56" s="14"/>
@@ -12932,7 +12938,7 @@
       </c>
       <c r="G58" s="14"/>
       <c r="H58" s="8" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="J58" s="14"/>
       <c r="K58" s="8" t="s">
@@ -13048,14 +13054,14 @@
       <c r="A61" s="7"/>
       <c r="D61" s="14"/>
       <c r="E61" s="8" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G61" s="14"/>
       <c r="H61" s="8" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J61" s="14"/>
       <c r="M61" s="23"/>
@@ -13198,10 +13204,7 @@
       </c>
       <c r="V64" s="14"/>
       <c r="W64" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="X64" s="8" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="Y64" s="14"/>
       <c r="Z64" s="27"/>
@@ -13262,11 +13265,9 @@
         <v>194</v>
       </c>
       <c r="W65" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="X65" s="8" t="s">
-        <v>104</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="X65" s="8"/>
       <c r="Z65" s="27"/>
       <c r="AA65" s="16"/>
       <c r="AB65" s="16"/>
@@ -13312,7 +13313,7 @@
         <v>217</v>
       </c>
       <c r="Q66" s="8" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="R66" s="8" t="s">
         <v>291</v>
@@ -13324,11 +13325,9 @@
         <v>195</v>
       </c>
       <c r="W66" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="X66" s="8" t="s">
-        <v>105</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="X66" s="8"/>
     </row>
     <row r="67" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
@@ -13352,22 +13351,20 @@
         <v>121</v>
       </c>
       <c r="O67" s="8" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="Q67" s="8"/>
       <c r="R67" s="8"/>
       <c r="T67" s="8" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="U67" s="8" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="W67" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="X67" s="8" t="s">
-        <v>111</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="X67" s="8"/>
     </row>
     <row r="68" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
@@ -13400,11 +13397,9 @@
       </c>
       <c r="U68" s="8"/>
       <c r="W68" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="X68" s="8" t="s">
-        <v>109</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="X68" s="8"/>
     </row>
     <row r="69" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
@@ -13426,20 +13421,18 @@
         <v>120</v>
       </c>
       <c r="O69" s="8" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="Q69" s="8"/>
       <c r="R69" s="8"/>
       <c r="T69" s="8" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="U69" s="8"/>
       <c r="W69" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="X69" s="8" t="s">
-        <v>110</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="X69" s="8"/>
     </row>
     <row r="70" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
@@ -13457,7 +13450,7 @@
         <v>211</v>
       </c>
       <c r="O70" s="8" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="Q70" s="8"/>
       <c r="R70" s="8"/>
@@ -13465,7 +13458,9 @@
         <v>289</v>
       </c>
       <c r="U70" s="8"/>
-      <c r="W70" s="8"/>
+      <c r="W70" s="8" t="s">
+        <v>111</v>
+      </c>
       <c r="X70" s="8"/>
     </row>
     <row r="71" spans="1:36" x14ac:dyDescent="0.25">
@@ -13482,7 +13477,7 @@
       <c r="L71" s="8"/>
       <c r="N71" s="8"/>
       <c r="O71" s="8" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="Q71" s="8"/>
       <c r="R71" s="8"/>
@@ -13490,7 +13485,9 @@
         <v>290</v>
       </c>
       <c r="U71" s="8"/>
-      <c r="W71" s="8"/>
+      <c r="W71" s="8" t="s">
+        <v>109</v>
+      </c>
       <c r="X71" s="8"/>
     </row>
     <row r="72" spans="1:36" x14ac:dyDescent="0.25">
@@ -13507,7 +13504,7 @@
       <c r="L72" s="8"/>
       <c r="N72" s="8"/>
       <c r="O72" s="8" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="Q72" s="8"/>
       <c r="R72" s="8"/>
@@ -13515,7 +13512,9 @@
         <v>291</v>
       </c>
       <c r="U72" s="8"/>
-      <c r="W72" s="8"/>
+      <c r="W72" s="8" t="s">
+        <v>110</v>
+      </c>
       <c r="X72" s="8"/>
     </row>
     <row r="73" spans="1:36" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Shrine, Planning and Scene updated
</commit_message>
<xml_diff>
--- a/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
+++ b/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
@@ -10497,8 +10497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q37" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="R65" sqref="R65"/>
+    <sheetView tabSelected="1" topLeftCell="Q28" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="T43" sqref="T43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
kappa kart terrain update
</commit_message>
<xml_diff>
--- a/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
+++ b/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enra\Documents\KoolKappaKlan\Concept\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aliek\OneDrive\Documenten\KoolKappaKlan\Concept\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2189" uniqueCount="723">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2190" uniqueCount="723">
   <si>
     <t>Arne</t>
   </si>
@@ -2200,7 +2200,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -2470,6 +2470,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2505,6 +2522,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -10497,8 +10531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q37" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="R65" sqref="R65"/>
+    <sheetView tabSelected="1" topLeftCell="Q21" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
+      <selection activeCell="U50" sqref="U50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12611,7 +12645,7 @@
         <v>332</v>
       </c>
       <c r="U51" s="8" t="s">
-        <v>338</v>
+        <v>96</v>
       </c>
       <c r="V51" s="14"/>
       <c r="Y51" s="14"/>
@@ -12647,6 +12681,9 @@
       <c r="S52" s="14"/>
       <c r="T52" s="8" t="s">
         <v>721</v>
+      </c>
+      <c r="U52" s="8" t="s">
+        <v>338</v>
       </c>
       <c r="V52" s="14"/>
       <c r="Y52" s="14"/>

</xml_diff>